<commit_message>
refactored to extract date from filename or data
</commit_message>
<xml_diff>
--- a/Leerplanillacupos/output_010324.xlsx
+++ b/Leerplanillacupos/output_010324.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -537,10 +541,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K2" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="3">
@@ -590,10 +592,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K3" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="4">
@@ -643,10 +643,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K4" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="5">
@@ -696,10 +694,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K5" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="6">
@@ -749,10 +745,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K6" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="7">
@@ -802,10 +796,8 @@
           <t>30</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K7" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="8">
@@ -855,10 +847,8 @@
           <t>26</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K8" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="9">
@@ -908,10 +898,8 @@
           <t>28</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K9" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="10">
@@ -961,10 +949,8 @@
           <t>25</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K10" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="11">
@@ -1014,10 +1000,8 @@
           <t>32</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K11" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="12">
@@ -1067,10 +1051,8 @@
           <t>31</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K12" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="13">
@@ -1120,10 +1102,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K13" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="14">
@@ -1173,10 +1153,8 @@
           <t>29</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K14" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="15">
@@ -1226,10 +1204,8 @@
           <t>30</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K15" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="16">
@@ -1279,10 +1255,8 @@
           <t>29</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K16" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="17">
@@ -1332,10 +1306,8 @@
           <t>35</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K17" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="18">
@@ -1385,10 +1357,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K18" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="19">
@@ -1438,10 +1408,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K19" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="20">
@@ -1491,10 +1459,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K20" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="21">
@@ -1544,10 +1510,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K21" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="22">
@@ -1597,10 +1561,8 @@
           <t>32</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K22" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="23">
@@ -1650,10 +1612,8 @@
           <t>30</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K23" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="24">
@@ -1703,10 +1663,8 @@
           <t>30</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K24" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="25">
@@ -1756,10 +1714,8 @@
           <t>30</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K25" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="26">
@@ -1809,10 +1765,8 @@
           <t>35</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K26" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="27">
@@ -1862,10 +1816,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K27" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="28">
@@ -1915,10 +1867,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K28" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="29">
@@ -1968,10 +1918,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K29" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="30">
@@ -2021,10 +1969,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K30" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="31">
@@ -2074,10 +2020,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K31" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="32">
@@ -2127,10 +2071,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K32" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="33">
@@ -2180,10 +2122,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K33" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="34">
@@ -2233,10 +2173,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K34" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="35">
@@ -2286,10 +2224,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K35" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="36">
@@ -2339,10 +2275,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K36" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
     <row r="37">
@@ -2392,10 +2326,8 @@
           <t>æ</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>010324</t>
-        </is>
+      <c r="K37" s="2" t="n">
+        <v>45352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>